<commit_message>
Split NG nonpeaker into ST and CC and remove quality tier in elec input data (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EAA5C7-1C89-4D35-950C-D882EA550009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="30255" yWindow="480" windowWidth="23445" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Notes:</t>
   </si>
@@ -44,9 +57,6 @@
   </si>
   <si>
     <t>BDPbES BAU Dispatch Priority by Electricity Source</t>
-  </si>
-  <si>
-    <t>natural gas nonpeaker</t>
   </si>
   <si>
     <t>geothermal</t>
@@ -93,11 +103,17 @@
   <si>
     <t>Priority Order (dimensionless)</t>
   </si>
+  <si>
+    <t>natural gas steam turbine</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,6 +253,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -272,6 +305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,7 +497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -471,22 +521,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -496,23 +546,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AK17"/>
+  <dimension ref="A1:AK18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2">
         <v>2015</v>
@@ -625,7 +675,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -635,7 +685,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:AK9" si="0">$B2</f>
+        <f t="shared" ref="D2:AK10" si="0">$B2</f>
         <v>2</v>
       </c>
       <c r="E2">
@@ -773,13 +823,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:R12" si="1">$B3</f>
+        <f t="shared" ref="C3:R13" si="1">$B3</f>
         <v>2</v>
       </c>
       <c r="D3">
@@ -921,7 +971,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -931,145 +981,145 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="S4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S4:AK4" si="2">$B4</f>
         <v>2</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="V4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="W4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="X4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AJ4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AK4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1217,7 +1267,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1365,7 +1415,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1513,7 +1563,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1661,7 +1711,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1799,17 +1849,17 @@
         <v>2</v>
       </c>
       <c r="AJ9">
-        <f t="shared" ref="D9:AK17" si="2">$B9</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1819,293 +1869,293 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="S10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="T10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="V10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="W10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="X10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AJ10">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D10:AK18" si="3">$B10</f>
         <v>2</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="V11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="W11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="X11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2115,293 +2165,293 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="V12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="X12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <f>$B13</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="P13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="X13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2411,583 +2461,731 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="V14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C17" si="3">$B15</f>
+        <f>$B15</f>
         <v>2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C16:C18" si="4">$B16</f>
         <v>2</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="R16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="S16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="T16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="U16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="V16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AJ16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AK16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="M17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="R17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="S17">
-        <f t="shared" ref="S17:AK17" si="4">$B17</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="T17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AI17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AJ17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AK17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="U17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="W17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="X17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Y17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AA17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AB17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AC17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AD17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AE17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AF17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AG17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AH17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AI17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AJ17">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AK17">
-        <f t="shared" si="4"/>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" ref="S18:AK18" si="5">$B18</f>
+        <v>2</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AJ18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AK18">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>

</xml_diff>